<commit_message>
35 - Fill in "Plan van aanpak" ( https://italent.cloudapp.net:9443/ccm/web/projects/iTalent#action=com.ibm.team.workitem.viewWorkItem&id=35 )
</commit_message>
<xml_diff>
--- a/italent/documents/quality/TimeSpent.xlsx
+++ b/italent/documents/quality/TimeSpent.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27022"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18165" windowHeight="8175" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="11620" yWindow="0" windowWidth="21980" windowHeight="19820" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Import from RTC" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,11 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="240">
   <si>
     <t>Type</t>
   </si>
@@ -746,6 +748,9 @@
   </si>
   <si>
     <t>Adjust detail page</t>
+  </si>
+  <si>
+    <t>Unit testing</t>
   </si>
 </sst>
 </file>
@@ -870,8 +875,8 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Goed" xfId="1" builtinId="26"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -917,7 +922,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -954,7 +959,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1088,13 +1093,13 @@
                   <c:v>190.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>106.25</c:v>
+                  <c:v>112.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1146,7 +1151,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1176,7 +1181,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1190,7 +1195,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1227,7 +1232,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1361,13 +1366,13 @@
                   <c:v>181.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>93.25</c:v>
+                  <c:v>99.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55</c:v>
+                  <c:v>96.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1419,7 +1424,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1449,7 +1454,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1463,7 +1468,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1500,7 +1505,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1634,13 +1639,13 @@
                   <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1692,7 +1697,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1722,7 +1727,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1736,7 +1741,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1773,7 +1778,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1847,10 +1852,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>33</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>514.6</c:v>
+                  <c:v>561.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1902,7 +1907,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1932,7 +1937,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4362,7 +4367,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4397,7 +4402,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4574,7 +4579,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4588,18 +4593,18 @@
       <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="83.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="83.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4625,7 +4630,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -4651,7 +4656,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4677,7 +4682,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -4703,7 +4708,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -4729,7 +4734,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -4755,7 +4760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -4781,7 +4786,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -4807,7 +4812,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -4833,7 +4838,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4859,7 +4864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -4885,7 +4890,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -4911,7 +4916,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -4937,7 +4942,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -4963,7 +4968,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -4989,7 +4994,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -5015,7 +5020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -5041,7 +5046,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -5067,7 +5072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -5093,7 +5098,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -5119,7 +5124,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -5145,7 +5150,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -5171,7 +5176,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -5197,7 +5202,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -5223,7 +5228,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -5249,7 +5254,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -5275,7 +5280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -5301,7 +5306,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -5327,7 +5332,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -5353,7 +5358,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -5379,7 +5384,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -5405,7 +5410,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -5431,7 +5436,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -5457,7 +5462,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -5483,7 +5488,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -5509,7 +5514,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -5535,7 +5540,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -5561,7 +5566,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -5587,7 +5592,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -5613,7 +5618,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -5639,7 +5644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -5665,7 +5670,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -5691,7 +5696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -5717,7 +5722,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>35</v>
       </c>
@@ -5743,7 +5748,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>35</v>
       </c>
@@ -5769,7 +5774,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>35</v>
       </c>
@@ -5795,7 +5800,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>35</v>
       </c>
@@ -5821,7 +5826,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>35</v>
       </c>
@@ -5847,7 +5852,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -5873,7 +5878,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -5899,7 +5904,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>35</v>
       </c>
@@ -5925,7 +5930,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -5951,7 +5956,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>35</v>
       </c>
@@ -5977,7 +5982,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>35</v>
       </c>
@@ -6003,7 +6008,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>35</v>
       </c>
@@ -6029,7 +6034,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>35</v>
       </c>
@@ -6055,7 +6060,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -6081,7 +6086,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -6107,7 +6112,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -6133,7 +6138,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>35</v>
       </c>
@@ -6159,7 +6164,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -6185,7 +6190,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -6211,7 +6216,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>8</v>
       </c>
@@ -6237,7 +6242,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -6263,7 +6268,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -6289,7 +6294,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -6315,7 +6320,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -6341,7 +6346,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -6367,7 +6372,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -6393,7 +6398,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -6419,7 +6424,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -6445,7 +6450,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -6471,7 +6476,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" t="s">
         <v>92</v>
       </c>
@@ -6497,7 +6502,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -6523,7 +6528,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>92</v>
       </c>
@@ -6549,7 +6554,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -6575,7 +6580,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -6601,7 +6606,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -6627,7 +6632,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -6653,7 +6658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>8</v>
       </c>
@@ -6679,7 +6684,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -6705,7 +6710,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" t="s">
         <v>8</v>
       </c>
@@ -6731,7 +6736,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -6757,7 +6762,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -6783,7 +6788,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>8</v>
       </c>
@@ -6809,7 +6814,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -6835,7 +6840,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
         <v>92</v>
       </c>
@@ -6861,7 +6866,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>8</v>
       </c>
@@ -6887,7 +6892,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>8</v>
       </c>
@@ -6913,7 +6918,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" t="s">
         <v>8</v>
       </c>
@@ -6939,7 +6944,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" t="s">
         <v>8</v>
       </c>
@@ -6965,7 +6970,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -6991,7 +6996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -7017,7 +7022,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" t="s">
         <v>8</v>
       </c>
@@ -7043,7 +7048,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" t="s">
         <v>8</v>
       </c>
@@ -7069,7 +7074,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" t="s">
         <v>8</v>
       </c>
@@ -7095,7 +7100,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" t="s">
         <v>8</v>
       </c>
@@ -7121,7 +7126,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" t="s">
         <v>8</v>
       </c>
@@ -7147,7 +7152,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" t="s">
         <v>8</v>
       </c>
@@ -7173,7 +7178,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" t="s">
         <v>92</v>
       </c>
@@ -7199,7 +7204,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8">
       <c r="A101" t="s">
         <v>8</v>
       </c>
@@ -7225,7 +7230,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8">
       <c r="A102" t="s">
         <v>8</v>
       </c>
@@ -7251,7 +7256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8">
       <c r="A103" t="s">
         <v>8</v>
       </c>
@@ -7277,7 +7282,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8">
       <c r="A104" t="s">
         <v>92</v>
       </c>
@@ -7303,7 +7308,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8">
       <c r="A105" t="s">
         <v>92</v>
       </c>
@@ -7329,7 +7334,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8">
       <c r="A106" t="s">
         <v>92</v>
       </c>
@@ -7355,7 +7360,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8">
       <c r="A107" t="s">
         <v>92</v>
       </c>
@@ -7381,7 +7386,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8">
       <c r="A108" t="s">
         <v>8</v>
       </c>
@@ -7407,7 +7412,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8">
       <c r="A109" t="s">
         <v>92</v>
       </c>
@@ -7433,7 +7438,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8">
       <c r="A110" t="s">
         <v>8</v>
       </c>
@@ -7459,7 +7464,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8">
       <c r="A111" t="s">
         <v>8</v>
       </c>
@@ -7485,7 +7490,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8">
       <c r="A112" t="s">
         <v>8</v>
       </c>
@@ -7511,7 +7516,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8">
       <c r="A113" t="s">
         <v>8</v>
       </c>
@@ -7537,7 +7542,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8">
       <c r="A114" t="s">
         <v>8</v>
       </c>
@@ -7563,7 +7568,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8">
       <c r="A115" t="s">
         <v>92</v>
       </c>
@@ -7589,7 +7594,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8">
       <c r="A116" t="s">
         <v>8</v>
       </c>
@@ -7615,7 +7620,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8">
       <c r="A117" t="s">
         <v>8</v>
       </c>
@@ -7641,7 +7646,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8">
       <c r="A118" t="s">
         <v>8</v>
       </c>
@@ -7667,7 +7672,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8">
       <c r="A119" t="s">
         <v>8</v>
       </c>
@@ -7693,7 +7698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8">
       <c r="A120" t="s">
         <v>8</v>
       </c>
@@ -7719,7 +7724,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8">
       <c r="A121" t="s">
         <v>8</v>
       </c>
@@ -7745,7 +7750,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8">
       <c r="A122" t="s">
         <v>8</v>
       </c>
@@ -7771,7 +7776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8">
       <c r="A123" t="s">
         <v>8</v>
       </c>
@@ -7797,7 +7802,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8">
       <c r="A124" t="s">
         <v>8</v>
       </c>
@@ -7823,7 +7828,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8">
       <c r="A125" t="s">
         <v>8</v>
       </c>
@@ -7849,7 +7854,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8">
       <c r="A126" t="s">
         <v>92</v>
       </c>
@@ -7875,7 +7880,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8">
       <c r="A127" t="s">
         <v>92</v>
       </c>
@@ -7901,7 +7906,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8">
       <c r="A128" t="s">
         <v>8</v>
       </c>
@@ -7927,7 +7932,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8">
       <c r="A129" t="s">
         <v>8</v>
       </c>
@@ -7953,7 +7958,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8">
       <c r="A130" t="s">
         <v>8</v>
       </c>
@@ -7979,7 +7984,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8">
       <c r="A131" t="s">
         <v>8</v>
       </c>
@@ -8005,7 +8010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8">
       <c r="A132" t="s">
         <v>92</v>
       </c>
@@ -8031,7 +8036,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8">
       <c r="A133" t="s">
         <v>8</v>
       </c>
@@ -8057,7 +8062,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8">
       <c r="A134" t="s">
         <v>92</v>
       </c>
@@ -8083,7 +8088,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8">
       <c r="A135" t="s">
         <v>92</v>
       </c>
@@ -8109,7 +8114,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8">
       <c r="A136" t="s">
         <v>8</v>
       </c>
@@ -8135,7 +8140,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8">
       <c r="A137" t="s">
         <v>92</v>
       </c>
@@ -8161,7 +8166,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8">
       <c r="A138" t="s">
         <v>8</v>
       </c>
@@ -8187,7 +8192,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8">
       <c r="A139" t="s">
         <v>8</v>
       </c>
@@ -8213,7 +8218,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8">
       <c r="A140" t="s">
         <v>8</v>
       </c>
@@ -8239,7 +8244,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8">
       <c r="A141" t="s">
         <v>8</v>
       </c>
@@ -8265,7 +8270,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8">
       <c r="A142" t="s">
         <v>92</v>
       </c>
@@ -8291,7 +8296,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8">
       <c r="A143" t="s">
         <v>8</v>
       </c>
@@ -8317,7 +8322,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8">
       <c r="A144" t="s">
         <v>92</v>
       </c>
@@ -8343,7 +8348,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8">
       <c r="A145" t="s">
         <v>8</v>
       </c>
@@ -8369,7 +8374,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8">
       <c r="A146" t="s">
         <v>8</v>
       </c>
@@ -8395,7 +8400,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8">
       <c r="A147" t="s">
         <v>92</v>
       </c>
@@ -8421,7 +8426,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8">
       <c r="A148" t="s">
         <v>8</v>
       </c>
@@ -8447,7 +8452,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8">
       <c r="A149" t="s">
         <v>8</v>
       </c>
@@ -8473,7 +8478,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8">
       <c r="A150" t="s">
         <v>8</v>
       </c>
@@ -8499,7 +8504,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8">
       <c r="A151" t="s">
         <v>8</v>
       </c>
@@ -8525,7 +8530,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8">
       <c r="A152" t="s">
         <v>92</v>
       </c>
@@ -8551,7 +8556,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8">
       <c r="A153" t="s">
         <v>8</v>
       </c>
@@ -8577,7 +8582,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8">
       <c r="A154" t="s">
         <v>8</v>
       </c>
@@ -8603,7 +8608,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8">
       <c r="A155" t="s">
         <v>92</v>
       </c>
@@ -8629,7 +8634,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8">
       <c r="A156" t="s">
         <v>8</v>
       </c>
@@ -8655,7 +8660,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8">
       <c r="A157" t="s">
         <v>8</v>
       </c>
@@ -8681,7 +8686,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8">
       <c r="A158" t="s">
         <v>8</v>
       </c>
@@ -8707,7 +8712,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8">
       <c r="A159" t="s">
         <v>92</v>
       </c>
@@ -8733,7 +8738,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8">
       <c r="A160" t="s">
         <v>8</v>
       </c>
@@ -8759,7 +8764,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8">
       <c r="A161" t="s">
         <v>8</v>
       </c>
@@ -8785,7 +8790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8">
       <c r="A162" t="s">
         <v>8</v>
       </c>
@@ -8811,7 +8816,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8">
       <c r="A163" t="s">
         <v>8</v>
       </c>
@@ -8837,7 +8842,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8">
       <c r="A164" t="s">
         <v>8</v>
       </c>
@@ -8863,7 +8868,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8">
       <c r="A165" t="s">
         <v>92</v>
       </c>
@@ -8889,7 +8894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8">
       <c r="A166" t="s">
         <v>92</v>
       </c>
@@ -8915,7 +8920,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8">
       <c r="A167" t="s">
         <v>92</v>
       </c>
@@ -8941,7 +8946,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8">
       <c r="A168" t="s">
         <v>92</v>
       </c>
@@ -8967,7 +8972,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8">
       <c r="A169" t="s">
         <v>92</v>
       </c>
@@ -8993,7 +8998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8">
       <c r="A170" t="s">
         <v>92</v>
       </c>
@@ -9019,7 +9024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8">
       <c r="A171" t="s">
         <v>92</v>
       </c>
@@ -9045,7 +9050,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8">
       <c r="A172" t="s">
         <v>8</v>
       </c>
@@ -9071,7 +9076,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8">
       <c r="A173" t="s">
         <v>92</v>
       </c>
@@ -9097,7 +9102,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8">
       <c r="A174" t="s">
         <v>92</v>
       </c>
@@ -9123,7 +9128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8">
       <c r="A175" t="s">
         <v>92</v>
       </c>
@@ -9149,7 +9154,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8">
       <c r="A176" t="s">
         <v>92</v>
       </c>
@@ -9175,7 +9180,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8">
       <c r="A177" t="s">
         <v>8</v>
       </c>
@@ -9201,7 +9206,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8">
       <c r="A178" t="s">
         <v>8</v>
       </c>
@@ -9227,7 +9232,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8">
       <c r="A179" t="s">
         <v>8</v>
       </c>
@@ -9253,7 +9258,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8">
       <c r="A180" t="s">
         <v>8</v>
       </c>
@@ -9279,7 +9284,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8">
       <c r="A181" t="s">
         <v>8</v>
       </c>
@@ -9305,7 +9310,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8">
       <c r="A182" t="s">
         <v>8</v>
       </c>
@@ -9331,7 +9336,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8">
       <c r="A183" t="s">
         <v>8</v>
       </c>
@@ -9357,7 +9362,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8">
       <c r="A184" t="s">
         <v>8</v>
       </c>
@@ -9383,7 +9388,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8">
       <c r="A185" t="s">
         <v>8</v>
       </c>
@@ -9409,7 +9414,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8">
       <c r="A186" t="s">
         <v>8</v>
       </c>
@@ -9435,7 +9440,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8">
       <c r="A187" t="s">
         <v>8</v>
       </c>
@@ -9461,7 +9466,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8">
       <c r="A188" t="s">
         <v>8</v>
       </c>
@@ -9487,7 +9492,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8">
       <c r="A189" t="s">
         <v>8</v>
       </c>
@@ -9513,7 +9518,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8">
       <c r="A190" t="s">
         <v>8</v>
       </c>
@@ -9539,7 +9544,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8">
       <c r="A191" t="s">
         <v>8</v>
       </c>
@@ -9565,7 +9570,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8">
       <c r="A192" t="s">
         <v>8</v>
       </c>
@@ -9591,7 +9596,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8">
       <c r="A193" t="s">
         <v>8</v>
       </c>
@@ -9617,7 +9622,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8">
       <c r="A194" t="s">
         <v>8</v>
       </c>
@@ -9643,7 +9648,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8">
       <c r="A195" t="s">
         <v>8</v>
       </c>
@@ -9669,7 +9674,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8">
       <c r="A196" t="s">
         <v>8</v>
       </c>
@@ -9695,7 +9700,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8">
       <c r="A197" t="s">
         <v>8</v>
       </c>
@@ -9721,7 +9726,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8">
       <c r="A198" t="s">
         <v>8</v>
       </c>
@@ -9747,7 +9752,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8">
       <c r="A199" t="s">
         <v>8</v>
       </c>
@@ -9773,7 +9778,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8">
       <c r="A200" t="s">
         <v>8</v>
       </c>
@@ -9799,7 +9804,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8">
       <c r="A201" t="s">
         <v>8</v>
       </c>
@@ -9825,7 +9830,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8">
       <c r="A202" t="s">
         <v>8</v>
       </c>
@@ -9851,7 +9856,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8">
       <c r="A203" t="s">
         <v>8</v>
       </c>
@@ -9879,6 +9884,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9886,23 +9896,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F110" sqref="F110"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="83.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="83.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="3" customFormat="1">
       <c r="B2" s="3" t="s">
         <v>227</v>
       </c>
@@ -9925,7 +9935,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="str">
         <f>'Import from RTC'!A73</f>
         <v>Defect</v>
@@ -9938,8 +9948,11 @@
         <f>'Import from RTC'!G91</f>
         <v>Dennie Grondelaers</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="str">
         <f>'Import from RTC'!A75</f>
         <v>Defect</v>
@@ -9956,7 +9969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" t="str">
         <f>'Import from RTC'!A84</f>
         <v>Defect</v>
@@ -9973,7 +9986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="str">
         <f>'Import from RTC'!A87</f>
         <v>Defect</v>
@@ -9987,7 +10000,7 @@
         <v>Niek Vandael</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="str">
         <f>'Import from RTC'!A100</f>
         <v>Defect</v>
@@ -10004,7 +10017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" t="str">
         <f>'Import from RTC'!A104</f>
         <v>Defect</v>
@@ -10021,7 +10034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" t="str">
         <f>'Import from RTC'!A105</f>
         <v>Defect</v>
@@ -10038,7 +10051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" t="str">
         <f>'Import from RTC'!A106</f>
         <v>Defect</v>
@@ -10055,7 +10068,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="str">
         <f>'Import from RTC'!A107</f>
         <v>Defect</v>
@@ -10072,7 +10085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" t="str">
         <f>'Import from RTC'!A109</f>
         <v>Defect</v>
@@ -10089,7 +10102,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" t="str">
         <f>'Import from RTC'!A115</f>
         <v>Defect</v>
@@ -10106,7 +10119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" t="str">
         <f>'Import from RTC'!A126</f>
         <v>Defect</v>
@@ -10123,7 +10136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" t="str">
         <f>'Import from RTC'!A127</f>
         <v>Defect</v>
@@ -10140,7 +10153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" t="str">
         <f>'Import from RTC'!A132</f>
         <v>Defect</v>
@@ -10157,7 +10170,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="str">
         <f>'Import from RTC'!A134</f>
         <v>Defect</v>
@@ -10174,7 +10187,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="str">
         <f>'Import from RTC'!A135</f>
         <v>Defect</v>
@@ -10188,7 +10201,7 @@
         <v>Niek Vandael</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" t="str">
         <f>'Import from RTC'!A137</f>
         <v>Defect</v>
@@ -10205,7 +10218,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" t="str">
         <f>'Import from RTC'!A142</f>
         <v>Defect</v>
@@ -10222,7 +10235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" t="str">
         <f>'Import from RTC'!A144</f>
         <v>Defect</v>
@@ -10239,7 +10252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" t="str">
         <f>'Import from RTC'!A147</f>
         <v>Defect</v>
@@ -10256,7 +10269,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" t="str">
         <f>'Import from RTC'!A152</f>
         <v>Defect</v>
@@ -10273,7 +10286,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" t="str">
         <f>'Import from RTC'!A155</f>
         <v>Defect</v>
@@ -10290,7 +10303,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" t="str">
         <f>'Import from RTC'!A159</f>
         <v>Defect</v>
@@ -10307,7 +10320,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" t="str">
         <f>'Import from RTC'!A165</f>
         <v>Defect</v>
@@ -10324,7 +10337,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" t="str">
         <f>'Import from RTC'!A166</f>
         <v>Defect</v>
@@ -10341,7 +10354,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" t="str">
         <f>'Import from RTC'!A167</f>
         <v>Defect</v>
@@ -10358,7 +10371,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" t="str">
         <f>'Import from RTC'!A168</f>
         <v>Defect</v>
@@ -10375,7 +10388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" t="str">
         <f>'Import from RTC'!A169</f>
         <v>Defect</v>
@@ -10392,7 +10405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" t="str">
         <f>'Import from RTC'!A170</f>
         <v>Defect</v>
@@ -10409,7 +10422,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" t="str">
         <f>'Import from RTC'!A171</f>
         <v>Defect</v>
@@ -10426,7 +10439,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" t="str">
         <f>'Import from RTC'!A173</f>
         <v>Defect</v>
@@ -10443,7 +10456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" t="str">
         <f>'Import from RTC'!A174</f>
         <v>Defect</v>
@@ -10460,7 +10473,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" t="str">
         <f>'Import from RTC'!A175</f>
         <v>Defect</v>
@@ -10477,7 +10490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" t="str">
         <f>'Import from RTC'!A176</f>
         <v>Defect</v>
@@ -10494,7 +10507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="2" customFormat="1">
       <c r="A38" s="2" t="s">
         <v>231</v>
       </c>
@@ -10512,7 +10525,7 @@
       </c>
       <c r="G38" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H38" s="2">
         <f t="shared" si="0"/>
@@ -10520,10 +10533,10 @@
       </c>
       <c r="I38">
         <f>SUM(D38:H38)</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" t="str">
         <f>'Import from RTC'!A2</f>
         <v>Task</v>
@@ -10540,7 +10553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" t="str">
         <f>'Import from RTC'!A3</f>
         <v>Task</v>
@@ -10557,7 +10570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" t="str">
         <f>'Import from RTC'!A4</f>
         <v>Task</v>
@@ -10574,7 +10587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44" t="str">
         <f>'Import from RTC'!A5</f>
         <v>Task</v>
@@ -10591,7 +10604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45" t="str">
         <f>'Import from RTC'!A6</f>
         <v>Task</v>
@@ -10608,7 +10621,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46" t="str">
         <f>'Import from RTC'!A7</f>
         <v>Task</v>
@@ -10625,7 +10638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" t="str">
         <f>'Import from RTC'!A8</f>
         <v>Task</v>
@@ -10642,7 +10655,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48" t="str">
         <f>'Import from RTC'!A10</f>
         <v>Task</v>
@@ -10662,7 +10675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" t="str">
         <f>'Import from RTC'!A11</f>
         <v>Task</v>
@@ -10682,7 +10695,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" t="str">
         <f>'Import from RTC'!A12</f>
         <v>Task</v>
@@ -10702,7 +10715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" t="str">
         <f>'Import from RTC'!A13</f>
         <v>Task</v>
@@ -10722,7 +10735,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" t="str">
         <f>'Import from RTC'!A14</f>
         <v>Task</v>
@@ -10751,7 +10764,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" t="str">
         <f>'Import from RTC'!A15</f>
         <v>Task</v>
@@ -10771,7 +10784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" t="str">
         <f>'Import from RTC'!A16</f>
         <v>Task</v>
@@ -10788,7 +10801,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" t="str">
         <f>'Import from RTC'!A17</f>
         <v>Task</v>
@@ -10805,7 +10818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" t="str">
         <f>'Import from RTC'!A18</f>
         <v>Task</v>
@@ -10828,7 +10841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" t="str">
         <f>'Import from RTC'!A20</f>
         <v>Task</v>
@@ -10857,7 +10870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" t="str">
         <f>'Import from RTC'!A21</f>
         <v>Task</v>
@@ -10886,7 +10899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" t="str">
         <f>'Import from RTC'!A22</f>
         <v>Task</v>
@@ -10906,7 +10919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" t="str">
         <f>'Import from RTC'!A24</f>
         <v>Task</v>
@@ -10923,7 +10936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" t="str">
         <f>'Import from RTC'!A25</f>
         <v>Task</v>
@@ -10943,7 +10956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" t="str">
         <f>'Import from RTC'!A26</f>
         <v>Task</v>
@@ -10972,7 +10985,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" t="str">
         <f>'Import from RTC'!A27</f>
         <v>Task</v>
@@ -10995,7 +11008,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" t="str">
         <f>'Import from RTC'!A29</f>
         <v>Task</v>
@@ -11015,7 +11028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" t="str">
         <f>'Import from RTC'!A30</f>
         <v>Task</v>
@@ -11032,7 +11045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" t="str">
         <f>'Import from RTC'!A31</f>
         <v>Task</v>
@@ -11049,7 +11062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" t="str">
         <f>'Import from RTC'!A33</f>
         <v>Task</v>
@@ -11072,7 +11085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" t="str">
         <f>'Import from RTC'!A34</f>
         <v>Task</v>
@@ -11089,7 +11102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" t="str">
         <f>'Import from RTC'!A39</f>
         <v>Task</v>
@@ -11115,7 +11128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" t="str">
         <f>'Import from RTC'!A40</f>
         <v>Task</v>
@@ -11135,7 +11148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" t="str">
         <f>'Import from RTC'!A57</f>
         <v>Task</v>
@@ -11155,7 +11168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" t="str">
         <f>'Import from RTC'!A58</f>
         <v>Task</v>
@@ -11172,7 +11185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" t="str">
         <f>'Import from RTC'!A59</f>
         <v>Task</v>
@@ -11189,7 +11202,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" t="str">
         <f>'Import from RTC'!A61</f>
         <v>Task</v>
@@ -11206,7 +11219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" t="str">
         <f>'Import from RTC'!A62</f>
         <v>Task</v>
@@ -11228,8 +11241,11 @@
       <c r="F75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" t="str">
         <f>'Import from RTC'!A63</f>
         <v>Task</v>
@@ -11246,7 +11262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" t="str">
         <f>'Import from RTC'!A64</f>
         <v>Task</v>
@@ -11263,7 +11279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" t="str">
         <f>'Import from RTC'!A65</f>
         <v>Task</v>
@@ -11280,7 +11296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" t="str">
         <f>'Import from RTC'!A66</f>
         <v>Task</v>
@@ -11297,7 +11313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" t="str">
         <f>'Import from RTC'!A67</f>
         <v>Task</v>
@@ -11311,10 +11327,13 @@
         <v>Dennie Grondelaers</v>
       </c>
       <c r="F80">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G80">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" t="str">
         <f>'Import from RTC'!A68</f>
         <v>Task</v>
@@ -11334,7 +11353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" t="str">
         <f>'Import from RTC'!A69</f>
         <v>Task</v>
@@ -11351,7 +11370,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" t="str">
         <f>'Import from RTC'!A70</f>
         <v>Task</v>
@@ -11368,7 +11387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" t="str">
         <f>'Import from RTC'!A71</f>
         <v>Task</v>
@@ -11385,7 +11404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" t="str">
         <f>'Import from RTC'!A72</f>
         <v>Task</v>
@@ -11402,7 +11421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" t="str">
         <f>'Import from RTC'!A74</f>
         <v>Task</v>
@@ -11419,7 +11438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87" t="str">
         <f>'Import from RTC'!A76</f>
         <v>Task</v>
@@ -11436,7 +11455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" t="str">
         <f>'Import from RTC'!A77</f>
         <v>Task</v>
@@ -11453,7 +11472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" t="str">
         <f>'Import from RTC'!A78</f>
         <v>Task</v>
@@ -11470,7 +11489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" t="str">
         <f>'Import from RTC'!A79</f>
         <v>Task</v>
@@ -11487,7 +11506,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" t="str">
         <f>'Import from RTC'!A80</f>
         <v>Task</v>
@@ -11504,7 +11523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" t="str">
         <f>'Import from RTC'!A81</f>
         <v>Task</v>
@@ -11521,7 +11540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" t="str">
         <f>'Import from RTC'!A82</f>
         <v>Task</v>
@@ -11538,7 +11557,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" t="str">
         <f>'Import from RTC'!A83</f>
         <v>Task</v>
@@ -11555,7 +11574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" t="str">
         <f>'Import from RTC'!A85</f>
         <v>Task</v>
@@ -11572,7 +11591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" t="str">
         <f>'Import from RTC'!A86</f>
         <v>Task</v>
@@ -11589,7 +11608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7">
       <c r="A97" t="str">
         <f>'Import from RTC'!A88</f>
         <v>Task</v>
@@ -11606,7 +11625,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7">
       <c r="A98" t="str">
         <f>'Import from RTC'!A89</f>
         <v>Task</v>
@@ -11623,7 +11642,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7">
       <c r="A99" t="str">
         <f>'Import from RTC'!A90</f>
         <v>Task</v>
@@ -11640,7 +11659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7">
       <c r="A100" t="str">
         <f>'Import from RTC'!A91</f>
         <v>Task</v>
@@ -11657,7 +11676,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7">
       <c r="A101" t="str">
         <f>'Import from RTC'!A92</f>
         <v>Task</v>
@@ -11674,7 +11693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7">
       <c r="A102" t="str">
         <f>'Import from RTC'!A93</f>
         <v>Task</v>
@@ -11691,7 +11710,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7">
       <c r="A103" t="str">
         <f>'Import from RTC'!A94</f>
         <v>Task</v>
@@ -11708,7 +11727,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7">
       <c r="A104" t="str">
         <f>'Import from RTC'!A95</f>
         <v>Task</v>
@@ -11725,7 +11744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7">
       <c r="A105" t="str">
         <f>'Import from RTC'!A96</f>
         <v>Task</v>
@@ -11742,7 +11761,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7">
       <c r="A106" t="str">
         <f>'Import from RTC'!A97</f>
         <v>Task</v>
@@ -11759,7 +11778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7">
       <c r="A107" t="str">
         <f>'Import from RTC'!A98</f>
         <v>Task</v>
@@ -11776,7 +11795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7">
       <c r="A108" t="str">
         <f>'Import from RTC'!A99</f>
         <v>Task</v>
@@ -11798,8 +11817,11 @@
       <c r="F108">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
       <c r="A109" t="str">
         <f>'Import from RTC'!A101</f>
         <v>Task</v>
@@ -11816,7 +11838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7">
       <c r="A110" t="str">
         <f>'Import from RTC'!A102</f>
         <v>Task</v>
@@ -11832,8 +11854,11 @@
       <c r="D110">
         <v>2</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
       <c r="A111" t="str">
         <f>'Import from RTC'!A103</f>
         <v>Task</v>
@@ -11850,7 +11875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7">
       <c r="A112" t="str">
         <f>'Import from RTC'!A108</f>
         <v>Task</v>
@@ -11867,7 +11892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6">
       <c r="A113" t="str">
         <f>'Import from RTC'!A110</f>
         <v>Task</v>
@@ -11884,7 +11909,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6">
       <c r="A114" t="str">
         <f>'Import from RTC'!A111</f>
         <v>Task</v>
@@ -11901,7 +11926,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6">
       <c r="A115" t="str">
         <f>'Import from RTC'!A112</f>
         <v>Task</v>
@@ -11918,7 +11943,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6">
       <c r="A116" t="str">
         <f>'Import from RTC'!A113</f>
         <v>Task</v>
@@ -11935,7 +11960,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6">
       <c r="A117" t="str">
         <f>'Import from RTC'!A114</f>
         <v>Task</v>
@@ -11952,7 +11977,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6">
       <c r="A118" t="str">
         <f>'Import from RTC'!A116</f>
         <v>Task</v>
@@ -11969,7 +11994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6">
       <c r="A119" t="str">
         <f>'Import from RTC'!A117</f>
         <v>Task</v>
@@ -11986,7 +12011,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6">
       <c r="A120" t="str">
         <f>'Import from RTC'!A118</f>
         <v>Task</v>
@@ -12003,7 +12028,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6">
       <c r="A121" t="str">
         <f>'Import from RTC'!A119</f>
         <v>Task</v>
@@ -12020,7 +12045,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6">
       <c r="A122" t="str">
         <f>'Import from RTC'!A120</f>
         <v>Task</v>
@@ -12037,7 +12062,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6">
       <c r="A123" t="str">
         <f>'Import from RTC'!A121</f>
         <v>Task</v>
@@ -12054,7 +12079,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6">
       <c r="A124" t="str">
         <f>'Import from RTC'!A122</f>
         <v>Task</v>
@@ -12068,7 +12093,7 @@
         <v>Niek Vandael</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6">
       <c r="A125" t="str">
         <f>'Import from RTC'!A123</f>
         <v>Task</v>
@@ -12085,7 +12110,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6">
       <c r="A126" t="str">
         <f>'Import from RTC'!A124</f>
         <v>Task</v>
@@ -12102,7 +12127,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6">
       <c r="A127" t="str">
         <f>'Import from RTC'!A125</f>
         <v>Task</v>
@@ -12119,7 +12144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6">
       <c r="A128" t="str">
         <f>'Import from RTC'!A128</f>
         <v>Task</v>
@@ -12136,7 +12161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5">
       <c r="A129" t="str">
         <f>'Import from RTC'!A129</f>
         <v>Task</v>
@@ -12153,7 +12178,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5">
       <c r="A130" t="str">
         <f>'Import from RTC'!A130</f>
         <v>Task</v>
@@ -12170,7 +12195,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5">
       <c r="A131" t="str">
         <f>'Import from RTC'!A131</f>
         <v>Task</v>
@@ -12187,7 +12212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5">
       <c r="A132" t="str">
         <f>'Import from RTC'!A133</f>
         <v>Task</v>
@@ -12204,7 +12229,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5">
       <c r="A133" t="str">
         <f>'Import from RTC'!A136</f>
         <v>Task</v>
@@ -12221,7 +12246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5">
       <c r="A134" t="str">
         <f>'Import from RTC'!A138</f>
         <v>Task</v>
@@ -12238,7 +12263,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5">
       <c r="A135" t="str">
         <f>'Import from RTC'!A139</f>
         <v>Task</v>
@@ -12255,7 +12280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5">
       <c r="A136" t="str">
         <f>'Import from RTC'!A140</f>
         <v>Task</v>
@@ -12272,7 +12297,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5">
       <c r="A137" t="str">
         <f>'Import from RTC'!A141</f>
         <v>Task</v>
@@ -12289,7 +12314,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5">
       <c r="A138" t="str">
         <f>'Import from RTC'!A143</f>
         <v>Task</v>
@@ -12306,7 +12331,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5">
       <c r="A139" t="str">
         <f>'Import from RTC'!A145</f>
         <v>Task</v>
@@ -12323,7 +12348,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5">
       <c r="A140" t="str">
         <f>'Import from RTC'!A146</f>
         <v>Task</v>
@@ -12340,7 +12365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5">
       <c r="A141" t="str">
         <f>'Import from RTC'!A148</f>
         <v>Task</v>
@@ -12357,7 +12382,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5">
       <c r="A142" t="str">
         <f>'Import from RTC'!A149</f>
         <v>Task</v>
@@ -12374,7 +12399,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5">
       <c r="A143" t="str">
         <f>'Import from RTC'!A150</f>
         <v>Task</v>
@@ -12391,7 +12416,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5">
       <c r="A144" t="str">
         <f>'Import from RTC'!A151</f>
         <v>Task</v>
@@ -12408,7 +12433,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6">
       <c r="A145" t="str">
         <f>'Import from RTC'!A153</f>
         <v>Task</v>
@@ -12425,7 +12450,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6">
       <c r="A146" t="str">
         <f>'Import from RTC'!A154</f>
         <v>Task</v>
@@ -12442,7 +12467,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6">
       <c r="A147" t="str">
         <f>'Import from RTC'!A156</f>
         <v>Task</v>
@@ -12459,7 +12484,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6">
       <c r="A148" t="str">
         <f>'Import from RTC'!A157</f>
         <v>Task</v>
@@ -12476,7 +12501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6">
       <c r="A149" t="str">
         <f>'Import from RTC'!A158</f>
         <v>Task</v>
@@ -12493,7 +12518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6">
       <c r="A150" t="str">
         <f>'Import from RTC'!A160</f>
         <v>Task</v>
@@ -12510,7 +12535,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6">
       <c r="A151" t="str">
         <f>'Import from RTC'!A161</f>
         <v>Task</v>
@@ -12527,7 +12552,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6">
       <c r="A152" t="str">
         <f>'Import from RTC'!A162</f>
         <v>Task</v>
@@ -12544,7 +12569,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6">
       <c r="A153" t="str">
         <f>'Import from RTC'!A163</f>
         <v>Task</v>
@@ -12561,7 +12586,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6">
       <c r="A154" t="str">
         <f>'Import from RTC'!A164</f>
         <v>Task</v>
@@ -12578,7 +12603,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6">
       <c r="A155" t="str">
         <f>'Import from RTC'!A172</f>
         <v>Task</v>
@@ -12595,7 +12620,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6">
       <c r="A156" t="str">
         <f>'Import from RTC'!A177</f>
         <v>Task</v>
@@ -12612,7 +12637,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6">
       <c r="A157" t="str">
         <f>'Import from RTC'!A178</f>
         <v>Task</v>
@@ -12629,7 +12654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6">
       <c r="A158" t="str">
         <f>'Import from RTC'!A179</f>
         <v>Task</v>
@@ -12646,7 +12671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6">
       <c r="A159" t="str">
         <f>'Import from RTC'!A180</f>
         <v>Task</v>
@@ -12663,7 +12688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6">
       <c r="A160" t="str">
         <f>'Import from RTC'!A181</f>
         <v>Task</v>
@@ -12680,7 +12705,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8">
       <c r="A161" t="str">
         <f>'Import from RTC'!A182</f>
         <v>Task</v>
@@ -12697,7 +12722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8">
       <c r="A162" t="str">
         <f>'Import from RTC'!A183</f>
         <v>Task</v>
@@ -12714,7 +12739,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8">
       <c r="A163" t="str">
         <f>'Import from RTC'!A184</f>
         <v>Task</v>
@@ -12731,7 +12756,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8">
       <c r="A164" t="s">
         <v>8</v>
       </c>
@@ -12759,7 +12784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8">
       <c r="A165" t="s">
         <v>8</v>
       </c>
@@ -12781,7 +12806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8">
       <c r="A166" t="s">
         <v>8</v>
       </c>
@@ -12803,7 +12828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8">
       <c r="A167" t="s">
         <v>8</v>
       </c>
@@ -12819,7 +12844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8">
       <c r="A168" t="s">
         <v>8</v>
       </c>
@@ -12832,7 +12857,7 @@
         <v>Unassigned</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8">
       <c r="A169" t="s">
         <v>8</v>
       </c>
@@ -12847,8 +12872,11 @@
       <c r="E169">
         <v>5</v>
       </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G169">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8">
       <c r="A170" t="s">
         <v>8</v>
       </c>
@@ -12867,7 +12895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8">
       <c r="A171" t="s">
         <v>8</v>
       </c>
@@ -12883,7 +12911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8">
       <c r="A172" t="s">
         <v>8</v>
       </c>
@@ -12899,7 +12927,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8">
       <c r="A173" t="s">
         <v>8</v>
       </c>
@@ -12915,7 +12943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8">
       <c r="A174" t="s">
         <v>8</v>
       </c>
@@ -12931,7 +12959,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8">
       <c r="A175" t="s">
         <v>8</v>
       </c>
@@ -12950,7 +12978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8">
       <c r="A176" t="s">
         <v>8</v>
       </c>
@@ -12972,7 +13000,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9">
       <c r="A177" t="s">
         <v>8</v>
       </c>
@@ -12988,7 +13016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9">
       <c r="A178" t="s">
         <v>8</v>
       </c>
@@ -13004,7 +13032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9">
       <c r="A179" t="s">
         <v>8</v>
       </c>
@@ -13020,7 +13048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9">
       <c r="A180" t="s">
         <v>8</v>
       </c>
@@ -13036,7 +13064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9">
       <c r="A181" t="s">
         <v>8</v>
       </c>
@@ -13052,7 +13080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9">
       <c r="A182" t="s">
         <v>8</v>
       </c>
@@ -13071,7 +13099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9">
       <c r="A183" t="s">
         <v>8</v>
       </c>
@@ -13087,7 +13115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9">
       <c r="A184" t="s">
         <v>8</v>
       </c>
@@ -13106,7 +13134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9">
       <c r="A185" t="s">
         <v>8</v>
       </c>
@@ -13118,8 +13146,11 @@
         <f>'Import from RTC'!G78</f>
         <v>Dennie Grondelaers</v>
       </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G185">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9">
       <c r="A186" t="s">
         <v>8</v>
       </c>
@@ -13137,8 +13168,11 @@
       <c r="E186">
         <v>5</v>
       </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G186">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9">
       <c r="A187" t="s">
         <v>8</v>
       </c>
@@ -13153,8 +13187,25 @@
       <c r="F187">
         <v>4</v>
       </c>
-    </row>
-    <row r="190" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9">
+      <c r="A188" t="s">
+        <v>8</v>
+      </c>
+      <c r="B188" t="s">
+        <v>239</v>
+      </c>
+      <c r="C188" t="s">
+        <v>30</v>
+      </c>
+      <c r="G188">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" s="2" customFormat="1">
       <c r="A190" s="2" t="s">
         <v>232</v>
       </c>
@@ -13168,11 +13219,11 @@
       </c>
       <c r="F190" s="2">
         <f>SUM(F41:F189)</f>
-        <v>93.25</v>
+        <v>99.25</v>
       </c>
       <c r="G190" s="2">
         <f>SUM(G41:G189)</f>
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="H190" s="2">
         <f>SUM(H41:H189)</f>
@@ -13180,10 +13231,10 @@
       </c>
       <c r="I190">
         <f>SUM(D190:H190)</f>
-        <v>514.6</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>561.6</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" s="2" customFormat="1">
       <c r="A194" s="2" t="s">
         <v>230</v>
       </c>
@@ -13192,24 +13243,24 @@
         <v>173.6</v>
       </c>
       <c r="E194" s="2">
-        <f t="shared" ref="E194:I194" si="1">E190+E38</f>
+        <f>E190+E38</f>
         <v>190.75</v>
       </c>
       <c r="F194" s="2">
-        <f t="shared" si="1"/>
-        <v>106.25</v>
+        <f>F190+F38</f>
+        <v>112.25</v>
       </c>
       <c r="G194" s="2">
-        <f t="shared" si="1"/>
-        <v>55</v>
+        <f>G190+G38</f>
+        <v>100</v>
       </c>
       <c r="H194" s="2">
-        <f t="shared" si="1"/>
+        <f>H190+H38</f>
         <v>22</v>
       </c>
       <c r="I194">
-        <f t="shared" si="1"/>
-        <v>547.6</v>
+        <f>I190+I38</f>
+        <v>598.6</v>
       </c>
     </row>
   </sheetData>
@@ -13217,7 +13268,12 @@
     <sortCondition ref="A3:A185"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -13229,17 +13285,17 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
         <v>228</v>
       </c>
@@ -13265,7 +13321,7 @@
       </c>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
         <v>230</v>
       </c>
@@ -13279,11 +13335,11 @@
       </c>
       <c r="D2" s="8">
         <f>'Time spent by user'!F194</f>
-        <v>106.25</v>
+        <v>112.25</v>
       </c>
       <c r="E2" s="8">
         <f>'Time spent by user'!G194</f>
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="F2" s="8">
         <f>'Time spent by user'!H194</f>
@@ -13293,6 +13349,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -13304,17 +13365,17 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
         <v>228</v>
       </c>
@@ -13339,7 +13400,7 @@
         <v>Bart Hunerbein</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="7" t="s">
         <v>232</v>
       </c>
@@ -13353,11 +13414,11 @@
       </c>
       <c r="D2" s="8">
         <f>'Time spent by user'!F190</f>
-        <v>93.25</v>
+        <v>99.25</v>
       </c>
       <c r="E2" s="8">
         <f>'Time spent by user'!G190</f>
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="F2" s="8">
         <f>'Time spent by user'!H190</f>
@@ -13367,6 +13428,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -13378,17 +13444,17 @@
       <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
         <v>228</v>
       </c>
@@ -13413,7 +13479,7 @@
         <v>Bart Hunerbein</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="7" t="s">
         <v>231</v>
       </c>
@@ -13431,7 +13497,7 @@
       </c>
       <c r="E2" s="8">
         <f>'Time spent by user'!G38</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F2" s="8">
         <f>'Time spent by user'!H38</f>
@@ -13441,6 +13507,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -13452,12 +13523,12 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -13468,22 +13539,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
         <v>233</v>
       </c>
       <c r="B2" s="8">
         <f>'Time spent by user'!I38</f>
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C2" s="8">
         <f>'Time spent by user'!I190</f>
-        <v>514.6</v>
+        <v>561.6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -13495,17 +13571,17 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7">
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="str">
         <f>'Time spent by user'!D2</f>
@@ -13528,7 +13604,7 @@
         <v>Bart Hunerbein</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7">
       <c r="B4" s="7" t="s">
         <v>229</v>
       </c>
@@ -13542,18 +13618,18 @@
       </c>
       <c r="E4" s="8">
         <f>'Total time spent'!D2</f>
-        <v>106.25</v>
+        <v>112.25</v>
       </c>
       <c r="F4" s="8">
         <f>'Total time spent'!E2</f>
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="G4" s="8">
         <f>'Total time spent'!F2</f>
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7">
       <c r="B5" s="9" t="s">
         <v>236</v>
       </c>
@@ -13573,7 +13649,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7">
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -13581,7 +13657,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7">
       <c r="B7" s="5" t="s">
         <v>237</v>
       </c>
@@ -13595,18 +13671,18 @@
       </c>
       <c r="E7" s="6">
         <f t="shared" si="0"/>
-        <v>2125</v>
+        <v>2245</v>
       </c>
       <c r="F7" s="6">
         <f t="shared" si="0"/>
-        <v>1100</v>
+        <v>2000</v>
       </c>
       <c r="G7" s="6">
         <f t="shared" si="0"/>
         <v>440</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7">
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -13614,7 +13690,7 @@
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7">
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -13622,13 +13698,13 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7">
       <c r="B10" s="7" t="s">
         <v>235</v>
       </c>
       <c r="C10" s="11">
         <f>SUM(C7:G7)</f>
-        <v>10952</v>
+        <v>11972</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -13637,6 +13713,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>